<commit_message>
Rename level to category
</commit_message>
<xml_diff>
--- a/inst/extdata/topics.xlsx
+++ b/inst/extdata/topics.xlsx
@@ -19,7 +19,7 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">level</t>
+    <t xml:space="preserve">category</t>
   </si>
   <si>
     <t xml:space="preserve">site</t>
@@ -34,22 +34,22 @@
     <t xml:space="preserve">Derek Maclellan</t>
   </si>
   <si>
-    <t xml:space="preserve">level_1</t>
+    <t xml:space="preserve">category_1</t>
   </si>
   <si>
     <t xml:space="preserve">site_1</t>
   </si>
   <si>
-    <t xml:space="preserve">level_2</t>
+    <t xml:space="preserve">category_2</t>
   </si>
   <si>
-    <t xml:space="preserve">level_3</t>
+    <t xml:space="preserve">category_3</t>
   </si>
   <si>
-    <t xml:space="preserve">level_4</t>
+    <t xml:space="preserve">category_4</t>
   </si>
   <si>
-    <t xml:space="preserve">level_5</t>
+    <t xml:space="preserve">category_5</t>
   </si>
   <si>
     <t xml:space="preserve">site_2</t>

</xml_diff>

<commit_message>
Rename site to option
</commit_message>
<xml_diff>
--- a/inst/extdata/topics.xlsx
+++ b/inst/extdata/topics.xlsx
@@ -22,7 +22,7 @@
     <t xml:space="preserve">category</t>
   </si>
   <si>
-    <t xml:space="preserve">site</t>
+    <t xml:space="preserve">option</t>
   </si>
   <si>
     <t xml:space="preserve">confidence</t>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">category_1</t>
   </si>
   <si>
-    <t xml:space="preserve">site_1</t>
+    <t xml:space="preserve">option_1</t>
   </si>
   <si>
     <t xml:space="preserve">category_2</t>
@@ -52,13 +52,13 @@
     <t xml:space="preserve">category_5</t>
   </si>
   <si>
-    <t xml:space="preserve">site_2</t>
+    <t xml:space="preserve">option_2</t>
   </si>
   <si>
-    <t xml:space="preserve">site_3</t>
+    <t xml:space="preserve">option_3</t>
   </si>
   <si>
-    <t xml:space="preserve">site_4</t>
+    <t xml:space="preserve">option_4</t>
   </si>
   <si>
     <t xml:space="preserve">Christopher Felix</t>

</xml_diff>

<commit_message>
Update order of parameters in elic_cat
(topic > option > category > ...)
</commit_message>
<xml_diff>
--- a/inst/extdata/topics.xlsx
+++ b/inst/extdata/topics.xlsx
@@ -19,10 +19,10 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">category</t>
+    <t xml:space="preserve">option</t>
   </si>
   <si>
-    <t xml:space="preserve">option</t>
+    <t xml:space="preserve">category</t>
   </si>
   <si>
     <t xml:space="preserve">confidence</t>
@@ -34,10 +34,10 @@
     <t xml:space="preserve">Derek Maclellan</t>
   </si>
   <si>
-    <t xml:space="preserve">category_1</t>
+    <t xml:space="preserve">option_1</t>
   </si>
   <si>
-    <t xml:space="preserve">option_1</t>
+    <t xml:space="preserve">category_1</t>
   </si>
   <si>
     <t xml:space="preserve">category_2</t>
@@ -444,10 +444,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>15</v>
@@ -461,10 +461,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>15</v>
@@ -478,10 +478,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>15</v>
@@ -495,10 +495,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
         <v>15</v>
@@ -512,10 +512,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
         <v>35</v>
@@ -529,10 +529,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
         <v>35</v>
@@ -546,10 +546,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>35</v>
@@ -563,10 +563,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>35</v>
@@ -580,10 +580,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
         <v>35</v>
@@ -597,10 +597,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>10</v>
@@ -614,10 +614,10 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
         <v>10</v>
@@ -631,10 +631,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
         <v>10</v>
@@ -648,10 +648,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
         <v>10</v>
@@ -665,10 +665,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
         <v>10</v>
@@ -682,10 +682,10 @@
         <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D17" t="n">
         <v>55</v>
@@ -699,10 +699,10 @@
         <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
         <v>55</v>
@@ -716,10 +716,10 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D19" t="n">
         <v>55</v>
@@ -733,10 +733,10 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
         <v>55</v>
@@ -750,10 +750,10 @@
         <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
         <v>55</v>
@@ -784,10 +784,10 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
         <v>65</v>
@@ -801,10 +801,10 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D24" t="n">
         <v>65</v>
@@ -818,10 +818,10 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D25" t="n">
         <v>65</v>
@@ -835,10 +835,10 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n">
         <v>65</v>
@@ -852,10 +852,10 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
         <v>80</v>
@@ -869,10 +869,10 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
         <v>80</v>
@@ -886,10 +886,10 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
         <v>80</v>
@@ -903,10 +903,10 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
         <v>80</v>
@@ -920,10 +920,10 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
         <v>80</v>
@@ -937,10 +937,10 @@
         <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D32" t="n">
         <v>55</v>
@@ -954,10 +954,10 @@
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n">
         <v>55</v>
@@ -971,10 +971,10 @@
         <v>15</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D34" t="n">
         <v>55</v>
@@ -988,10 +988,10 @@
         <v>15</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D35" t="n">
         <v>55</v>
@@ -1005,10 +1005,10 @@
         <v>15</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D36" t="n">
         <v>55</v>
@@ -1022,10 +1022,10 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D37" t="n">
         <v>40</v>
@@ -1039,10 +1039,10 @@
         <v>15</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D38" t="n">
         <v>40</v>
@@ -1056,10 +1056,10 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
         <v>40</v>
@@ -1073,10 +1073,10 @@
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D40" t="n">
         <v>40</v>
@@ -1090,10 +1090,10 @@
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D41" t="n">
         <v>40</v>
@@ -1124,10 +1124,10 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" t="n">
         <v>100</v>
@@ -1141,10 +1141,10 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D44" t="n">
         <v>100</v>
@@ -1158,10 +1158,10 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D45" t="n">
         <v>100</v>
@@ -1175,10 +1175,10 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D46" t="n">
         <v>100</v>
@@ -1192,10 +1192,10 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D47" t="n">
         <v>85</v>
@@ -1209,10 +1209,10 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D48" t="n">
         <v>85</v>
@@ -1226,10 +1226,10 @@
         <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D49" t="n">
         <v>85</v>
@@ -1243,10 +1243,10 @@
         <v>16</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D50" t="n">
         <v>85</v>
@@ -1260,10 +1260,10 @@
         <v>16</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
         <v>85</v>
@@ -1277,10 +1277,10 @@
         <v>16</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
         <v>75</v>
@@ -1294,10 +1294,10 @@
         <v>16</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D53" t="n">
         <v>75</v>
@@ -1311,10 +1311,10 @@
         <v>16</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D54" t="n">
         <v>75</v>
@@ -1328,10 +1328,10 @@
         <v>16</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D55" t="n">
         <v>75</v>
@@ -1345,10 +1345,10 @@
         <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D56" t="n">
         <v>75</v>
@@ -1362,10 +1362,10 @@
         <v>16</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D57" t="n">
         <v>65</v>
@@ -1379,10 +1379,10 @@
         <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D58" t="n">
         <v>65</v>
@@ -1396,10 +1396,10 @@
         <v>16</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D59" t="n">
         <v>65</v>
@@ -1413,10 +1413,10 @@
         <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D60" t="n">
         <v>65</v>
@@ -1430,10 +1430,10 @@
         <v>16</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D61" t="n">
         <v>65</v>
@@ -1464,10 +1464,10 @@
         <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
         <v>55</v>
@@ -1481,10 +1481,10 @@
         <v>17</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D64" t="n">
         <v>55</v>
@@ -1498,10 +1498,10 @@
         <v>17</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D65" t="n">
         <v>55</v>
@@ -1515,10 +1515,10 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D66" t="n">
         <v>55</v>
@@ -1532,10 +1532,10 @@
         <v>17</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D67" t="n">
         <v>35</v>
@@ -1549,10 +1549,10 @@
         <v>17</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D68" t="n">
         <v>35</v>
@@ -1566,10 +1566,10 @@
         <v>17</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D69" t="n">
         <v>35</v>
@@ -1583,10 +1583,10 @@
         <v>17</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D70" t="n">
         <v>35</v>
@@ -1600,10 +1600,10 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" t="n">
         <v>35</v>
@@ -1617,10 +1617,10 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D72" t="n">
         <v>40</v>
@@ -1634,10 +1634,10 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D73" t="n">
         <v>40</v>
@@ -1651,10 +1651,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D74" t="n">
         <v>40</v>
@@ -1668,10 +1668,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D75" t="n">
         <v>40</v>
@@ -1685,10 +1685,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D76" t="n">
         <v>40</v>
@@ -1702,10 +1702,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D77" t="n">
         <v>5</v>
@@ -1719,10 +1719,10 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D78" t="n">
         <v>5</v>
@@ -1736,10 +1736,10 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D79" t="n">
         <v>5</v>
@@ -1753,10 +1753,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D80" t="n">
         <v>5</v>
@@ -1770,10 +1770,10 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
         <v>5</v>
@@ -1804,10 +1804,10 @@
         <v>18</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D83" t="n">
         <v>40</v>
@@ -1821,10 +1821,10 @@
         <v>18</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D84" t="n">
         <v>40</v>
@@ -1838,10 +1838,10 @@
         <v>18</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D85" t="n">
         <v>40</v>
@@ -1855,10 +1855,10 @@
         <v>18</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D86" t="n">
         <v>40</v>
@@ -1872,10 +1872,10 @@
         <v>18</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D87" t="n">
         <v>90</v>
@@ -1889,10 +1889,10 @@
         <v>18</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D88" t="n">
         <v>90</v>
@@ -1906,10 +1906,10 @@
         <v>18</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D89" t="n">
         <v>90</v>
@@ -1923,10 +1923,10 @@
         <v>18</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D90" t="n">
         <v>90</v>
@@ -1940,10 +1940,10 @@
         <v>18</v>
       </c>
       <c r="B91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D91" t="n">
         <v>90</v>
@@ -1957,10 +1957,10 @@
         <v>18</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D92" t="n">
         <v>55</v>
@@ -1974,10 +1974,10 @@
         <v>18</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D93" t="n">
         <v>55</v>
@@ -1991,10 +1991,10 @@
         <v>18</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D94" t="n">
         <v>55</v>
@@ -2008,10 +2008,10 @@
         <v>18</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D95" t="n">
         <v>55</v>
@@ -2025,10 +2025,10 @@
         <v>18</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D96" t="n">
         <v>55</v>
@@ -2042,10 +2042,10 @@
         <v>18</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D97" t="n">
         <v>55</v>
@@ -2059,10 +2059,10 @@
         <v>18</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C98" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D98" t="n">
         <v>55</v>
@@ -2076,10 +2076,10 @@
         <v>18</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D99" t="n">
         <v>55</v>
@@ -2093,10 +2093,10 @@
         <v>18</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D100" t="n">
         <v>55</v>
@@ -2110,10 +2110,10 @@
         <v>18</v>
       </c>
       <c r="B101" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D101" t="n">
         <v>55</v>
@@ -2144,10 +2144,10 @@
         <v>19</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D103" t="n">
         <v>30</v>
@@ -2161,10 +2161,10 @@
         <v>19</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C104" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D104" t="n">
         <v>30</v>
@@ -2178,10 +2178,10 @@
         <v>19</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C105" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D105" t="n">
         <v>30</v>
@@ -2195,10 +2195,10 @@
         <v>19</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D106" t="n">
         <v>30</v>
@@ -2212,10 +2212,10 @@
         <v>19</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D107" t="n">
         <v>90</v>
@@ -2229,10 +2229,10 @@
         <v>19</v>
       </c>
       <c r="B108" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D108" t="n">
         <v>90</v>
@@ -2246,10 +2246,10 @@
         <v>19</v>
       </c>
       <c r="B109" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D109" t="n">
         <v>90</v>
@@ -2263,10 +2263,10 @@
         <v>19</v>
       </c>
       <c r="B110" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D110" t="n">
         <v>90</v>
@@ -2280,10 +2280,10 @@
         <v>19</v>
       </c>
       <c r="B111" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D111" t="n">
         <v>90</v>
@@ -2297,10 +2297,10 @@
         <v>19</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C112" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D112" t="n">
         <v>35</v>
@@ -2314,10 +2314,10 @@
         <v>19</v>
       </c>
       <c r="B113" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C113" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D113" t="n">
         <v>35</v>
@@ -2331,10 +2331,10 @@
         <v>19</v>
       </c>
       <c r="B114" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C114" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D114" t="n">
         <v>35</v>
@@ -2348,10 +2348,10 @@
         <v>19</v>
       </c>
       <c r="B115" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C115" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D115" t="n">
         <v>35</v>
@@ -2365,10 +2365,10 @@
         <v>19</v>
       </c>
       <c r="B116" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C116" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D116" t="n">
         <v>35</v>
@@ -2382,10 +2382,10 @@
         <v>19</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C117" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D117" t="n">
         <v>35</v>
@@ -2399,10 +2399,10 @@
         <v>19</v>
       </c>
       <c r="B118" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C118" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D118" t="n">
         <v>35</v>
@@ -2416,10 +2416,10 @@
         <v>19</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C119" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D119" t="n">
         <v>35</v>
@@ -2433,10 +2433,10 @@
         <v>19</v>
       </c>
       <c r="B120" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C120" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D120" t="n">
         <v>35</v>
@@ -2450,10 +2450,10 @@
         <v>19</v>
       </c>
       <c r="B121" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C121" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D121" t="n">
         <v>35</v>
@@ -2515,10 +2515,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>100</v>
@@ -2532,10 +2532,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>100</v>
@@ -2549,10 +2549,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>100</v>
@@ -2566,10 +2566,10 @@
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
         <v>100</v>
@@ -2583,10 +2583,10 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
         <v>20</v>
@@ -2600,10 +2600,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
         <v>20</v>
@@ -2617,10 +2617,10 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>20</v>
@@ -2634,10 +2634,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>20</v>
@@ -2651,10 +2651,10 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
         <v>20</v>
@@ -2668,10 +2668,10 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>85</v>
@@ -2685,10 +2685,10 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
         <v>85</v>
@@ -2702,10 +2702,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
         <v>85</v>
@@ -2719,10 +2719,10 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
         <v>85</v>
@@ -2736,10 +2736,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
         <v>85</v>
@@ -2753,10 +2753,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D17" t="n">
         <v>70</v>
@@ -2770,10 +2770,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
         <v>70</v>
@@ -2787,10 +2787,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D19" t="n">
         <v>70</v>
@@ -2804,10 +2804,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
         <v>70</v>
@@ -2821,10 +2821,10 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
         <v>70</v>
@@ -2855,10 +2855,10 @@
         <v>16</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
         <v>75</v>
@@ -2872,10 +2872,10 @@
         <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D24" t="n">
         <v>75</v>
@@ -2889,10 +2889,10 @@
         <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D25" t="n">
         <v>75</v>
@@ -2906,10 +2906,10 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n">
         <v>75</v>
@@ -2923,10 +2923,10 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
         <v>95</v>
@@ -2940,10 +2940,10 @@
         <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
         <v>95</v>
@@ -2957,10 +2957,10 @@
         <v>16</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
         <v>95</v>
@@ -2974,10 +2974,10 @@
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
         <v>95</v>
@@ -2991,10 +2991,10 @@
         <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
         <v>95</v>
@@ -3008,10 +3008,10 @@
         <v>16</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D32" t="n">
         <v>35</v>
@@ -3025,10 +3025,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n">
         <v>35</v>
@@ -3042,10 +3042,10 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D34" t="n">
         <v>35</v>
@@ -3059,10 +3059,10 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C35" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D35" t="n">
         <v>35</v>
@@ -3076,10 +3076,10 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D36" t="n">
         <v>35</v>
@@ -3093,10 +3093,10 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D37" t="n">
         <v>5</v>
@@ -3110,10 +3110,10 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D38" t="n">
         <v>5</v>
@@ -3127,10 +3127,10 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
         <v>5</v>
@@ -3144,10 +3144,10 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D40" t="n">
         <v>5</v>
@@ -3161,10 +3161,10 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D41" t="n">
         <v>5</v>
@@ -3195,10 +3195,10 @@
         <v>17</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D43" t="n">
         <v>100</v>
@@ -3212,10 +3212,10 @@
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D44" t="n">
         <v>100</v>
@@ -3229,10 +3229,10 @@
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D45" t="n">
         <v>100</v>
@@ -3246,10 +3246,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D46" t="n">
         <v>100</v>
@@ -3263,10 +3263,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D47" t="n">
         <v>100</v>
@@ -3280,10 +3280,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D48" t="n">
         <v>100</v>
@@ -3297,10 +3297,10 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D49" t="n">
         <v>100</v>
@@ -3314,10 +3314,10 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D50" t="n">
         <v>100</v>
@@ -3331,10 +3331,10 @@
         <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
         <v>100</v>
@@ -3348,10 +3348,10 @@
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
         <v>15</v>
@@ -3365,10 +3365,10 @@
         <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D53" t="n">
         <v>15</v>
@@ -3382,10 +3382,10 @@
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D54" t="n">
         <v>15</v>
@@ -3399,10 +3399,10 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C55" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D55" t="n">
         <v>15</v>
@@ -3416,10 +3416,10 @@
         <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D56" t="n">
         <v>15</v>
@@ -3433,10 +3433,10 @@
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D57" t="n">
         <v>25</v>
@@ -3450,10 +3450,10 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D58" t="n">
         <v>25</v>
@@ -3467,10 +3467,10 @@
         <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D59" t="n">
         <v>25</v>
@@ -3484,10 +3484,10 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C60" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D60" t="n">
         <v>25</v>
@@ -3501,10 +3501,10 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D61" t="n">
         <v>25</v>
@@ -3535,10 +3535,10 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
         <v>80</v>
@@ -3552,10 +3552,10 @@
         <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D64" t="n">
         <v>80</v>
@@ -3569,10 +3569,10 @@
         <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D65" t="n">
         <v>80</v>
@@ -3586,10 +3586,10 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D66" t="n">
         <v>80</v>
@@ -3603,10 +3603,10 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D67" t="n">
         <v>35</v>
@@ -3620,10 +3620,10 @@
         <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D68" t="n">
         <v>35</v>
@@ -3637,10 +3637,10 @@
         <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D69" t="n">
         <v>35</v>
@@ -3654,10 +3654,10 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D70" t="n">
         <v>35</v>
@@ -3671,10 +3671,10 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" t="n">
         <v>35</v>
@@ -3688,10 +3688,10 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D72" t="n">
         <v>15</v>
@@ -3705,10 +3705,10 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D73" t="n">
         <v>15</v>
@@ -3722,10 +3722,10 @@
         <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D74" t="n">
         <v>15</v>
@@ -3739,10 +3739,10 @@
         <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D75" t="n">
         <v>15</v>
@@ -3756,10 +3756,10 @@
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D76" t="n">
         <v>15</v>
@@ -3773,10 +3773,10 @@
         <v>18</v>
       </c>
       <c r="B77" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D77" t="n">
         <v>5</v>
@@ -3790,10 +3790,10 @@
         <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D78" t="n">
         <v>5</v>
@@ -3807,10 +3807,10 @@
         <v>18</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D79" t="n">
         <v>5</v>
@@ -3824,10 +3824,10 @@
         <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D80" t="n">
         <v>5</v>
@@ -3841,10 +3841,10 @@
         <v>18</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
         <v>5</v>
@@ -3875,10 +3875,10 @@
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D83" t="n">
         <v>15</v>
@@ -3892,10 +3892,10 @@
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C84" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D84" t="n">
         <v>15</v>
@@ -3909,10 +3909,10 @@
         <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D85" t="n">
         <v>15</v>
@@ -3926,10 +3926,10 @@
         <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C86" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D86" t="n">
         <v>15</v>
@@ -3943,10 +3943,10 @@
         <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D87" t="n">
         <v>5</v>
@@ -3960,10 +3960,10 @@
         <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D88" t="n">
         <v>5</v>
@@ -3977,10 +3977,10 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D89" t="n">
         <v>5</v>
@@ -3994,10 +3994,10 @@
         <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D90" t="n">
         <v>5</v>
@@ -4011,10 +4011,10 @@
         <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D91" t="n">
         <v>5</v>
@@ -4028,10 +4028,10 @@
         <v>19</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C92" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D92" t="n">
         <v>55</v>
@@ -4045,10 +4045,10 @@
         <v>19</v>
       </c>
       <c r="B93" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D93" t="n">
         <v>55</v>
@@ -4062,10 +4062,10 @@
         <v>19</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C94" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D94" t="n">
         <v>55</v>
@@ -4079,10 +4079,10 @@
         <v>19</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C95" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D95" t="n">
         <v>55</v>
@@ -4096,10 +4096,10 @@
         <v>19</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C96" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D96" t="n">
         <v>55</v>
@@ -4113,10 +4113,10 @@
         <v>19</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C97" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D97" t="n">
         <v>40</v>
@@ -4130,10 +4130,10 @@
         <v>19</v>
       </c>
       <c r="B98" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C98" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D98" t="n">
         <v>40</v>
@@ -4147,10 +4147,10 @@
         <v>19</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C99" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D99" t="n">
         <v>40</v>
@@ -4164,10 +4164,10 @@
         <v>19</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D100" t="n">
         <v>40</v>
@@ -4181,10 +4181,10 @@
         <v>19</v>
       </c>
       <c r="B101" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C101" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D101" t="n">
         <v>40</v>
@@ -4246,10 +4246,10 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="n">
         <v>80</v>
@@ -4263,10 +4263,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>80</v>
@@ -4280,10 +4280,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>80</v>
@@ -4297,10 +4297,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
         <v>80</v>
@@ -4314,10 +4314,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D7" t="n">
         <v>50</v>
@@ -4331,10 +4331,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D8" t="n">
         <v>50</v>
@@ -4348,10 +4348,10 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D9" t="n">
         <v>50</v>
@@ -4365,10 +4365,10 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D10" t="n">
         <v>50</v>
@@ -4382,10 +4382,10 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
         <v>50</v>
@@ -4399,10 +4399,10 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D12" t="n">
         <v>15</v>
@@ -4416,10 +4416,10 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D13" t="n">
         <v>15</v>
@@ -4433,10 +4433,10 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
         <v>15</v>
@@ -4450,10 +4450,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D15" t="n">
         <v>15</v>
@@ -4467,10 +4467,10 @@
         <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
         <v>15</v>
@@ -4501,10 +4501,10 @@
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" t="n">
         <v>25</v>
@@ -4518,10 +4518,10 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D19" t="n">
         <v>25</v>
@@ -4535,10 +4535,10 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D20" t="n">
         <v>25</v>
@@ -4552,10 +4552,10 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D21" t="n">
         <v>25</v>
@@ -4569,10 +4569,10 @@
         <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D22" t="n">
         <v>100</v>
@@ -4586,10 +4586,10 @@
         <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D23" t="n">
         <v>100</v>
@@ -4603,10 +4603,10 @@
         <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D24" t="n">
         <v>100</v>
@@ -4620,10 +4620,10 @@
         <v>15</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D25" t="n">
         <v>100</v>
@@ -4637,10 +4637,10 @@
         <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="n">
         <v>100</v>
@@ -4654,10 +4654,10 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D27" t="n">
         <v>55</v>
@@ -4671,10 +4671,10 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D28" t="n">
         <v>55</v>
@@ -4688,10 +4688,10 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D29" t="n">
         <v>55</v>
@@ -4705,10 +4705,10 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D30" t="n">
         <v>55</v>
@@ -4722,10 +4722,10 @@
         <v>15</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D31" t="n">
         <v>55</v>
@@ -4756,10 +4756,10 @@
         <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D33" t="n">
         <v>60</v>
@@ -4773,10 +4773,10 @@
         <v>16</v>
       </c>
       <c r="B34" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D34" t="n">
         <v>60</v>
@@ -4790,10 +4790,10 @@
         <v>16</v>
       </c>
       <c r="B35" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D35" t="n">
         <v>60</v>
@@ -4807,10 +4807,10 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D36" t="n">
         <v>60</v>
@@ -4824,10 +4824,10 @@
         <v>16</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D37" t="n">
         <v>15</v>
@@ -4841,10 +4841,10 @@
         <v>16</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D38" t="n">
         <v>15</v>
@@ -4858,10 +4858,10 @@
         <v>16</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D39" t="n">
         <v>15</v>
@@ -4875,10 +4875,10 @@
         <v>16</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D40" t="n">
         <v>15</v>
@@ -4892,10 +4892,10 @@
         <v>16</v>
       </c>
       <c r="B41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D41" t="n">
         <v>15</v>
@@ -4909,10 +4909,10 @@
         <v>16</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C42" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D42" t="n">
         <v>75</v>
@@ -4926,10 +4926,10 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D43" t="n">
         <v>75</v>
@@ -4943,10 +4943,10 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D44" t="n">
         <v>75</v>
@@ -4960,10 +4960,10 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D45" t="n">
         <v>75</v>
@@ -4977,10 +4977,10 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D46" t="n">
         <v>75</v>
@@ -5011,10 +5011,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D48" t="n">
         <v>100</v>
@@ -5028,10 +5028,10 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D49" t="n">
         <v>100</v>
@@ -5045,10 +5045,10 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D50" t="n">
         <v>100</v>
@@ -5062,10 +5062,10 @@
         <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
         <v>100</v>
@@ -5079,10 +5079,10 @@
         <v>17</v>
       </c>
       <c r="B52" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D52" t="n">
         <v>0</v>
@@ -5096,10 +5096,10 @@
         <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
@@ -5113,10 +5113,10 @@
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D54" t="n">
         <v>0</v>
@@ -5130,10 +5130,10 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D55" t="n">
         <v>0</v>
@@ -5147,10 +5147,10 @@
         <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -5164,10 +5164,10 @@
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D57" t="n">
         <v>70</v>
@@ -5181,10 +5181,10 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D58" t="n">
         <v>70</v>
@@ -5198,10 +5198,10 @@
         <v>17</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C59" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D59" t="n">
         <v>70</v>
@@ -5215,10 +5215,10 @@
         <v>17</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C60" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D60" t="n">
         <v>70</v>
@@ -5232,10 +5232,10 @@
         <v>17</v>
       </c>
       <c r="B61" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C61" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D61" t="n">
         <v>70</v>
@@ -5266,10 +5266,10 @@
         <v>18</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D63" t="n">
         <v>95</v>
@@ -5283,10 +5283,10 @@
         <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D64" t="n">
         <v>95</v>
@@ -5300,10 +5300,10 @@
         <v>18</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D65" t="n">
         <v>95</v>
@@ -5317,10 +5317,10 @@
         <v>18</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D66" t="n">
         <v>95</v>
@@ -5334,10 +5334,10 @@
         <v>18</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D67" t="n">
         <v>90</v>
@@ -5351,10 +5351,10 @@
         <v>18</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D68" t="n">
         <v>90</v>
@@ -5368,10 +5368,10 @@
         <v>18</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D69" t="n">
         <v>90</v>
@@ -5385,10 +5385,10 @@
         <v>18</v>
       </c>
       <c r="B70" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D70" t="n">
         <v>90</v>
@@ -5402,10 +5402,10 @@
         <v>18</v>
       </c>
       <c r="B71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D71" t="n">
         <v>90</v>
@@ -5419,10 +5419,10 @@
         <v>18</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C72" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D72" t="n">
         <v>55</v>
@@ -5436,10 +5436,10 @@
         <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D73" t="n">
         <v>55</v>
@@ -5453,10 +5453,10 @@
         <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D74" t="n">
         <v>55</v>
@@ -5470,10 +5470,10 @@
         <v>18</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D75" t="n">
         <v>55</v>
@@ -5487,10 +5487,10 @@
         <v>18</v>
       </c>
       <c r="B76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D76" t="n">
         <v>55</v>
@@ -5521,10 +5521,10 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D78" t="n">
         <v>75</v>
@@ -5538,10 +5538,10 @@
         <v>19</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C79" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D79" t="n">
         <v>75</v>
@@ -5555,10 +5555,10 @@
         <v>19</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D80" t="n">
         <v>75</v>
@@ -5572,10 +5572,10 @@
         <v>19</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
         <v>75</v>
@@ -5589,10 +5589,10 @@
         <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D82" t="n">
         <v>20</v>
@@ -5606,10 +5606,10 @@
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D83" t="n">
         <v>20</v>
@@ -5623,10 +5623,10 @@
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D84" t="n">
         <v>20</v>
@@ -5640,10 +5640,10 @@
         <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D85" t="n">
         <v>20</v>
@@ -5657,10 +5657,10 @@
         <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D86" t="n">
         <v>20</v>
@@ -5674,10 +5674,10 @@
         <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C87" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D87" t="n">
         <v>35</v>
@@ -5691,10 +5691,10 @@
         <v>19</v>
       </c>
       <c r="B88" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C88" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D88" t="n">
         <v>35</v>
@@ -5708,10 +5708,10 @@
         <v>19</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C89" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D89" t="n">
         <v>35</v>
@@ -5725,10 +5725,10 @@
         <v>19</v>
       </c>
       <c r="B90" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C90" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D90" t="n">
         <v>35</v>
@@ -5742,10 +5742,10 @@
         <v>19</v>
       </c>
       <c r="B91" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C91" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D91" t="n">
         <v>35</v>

</xml_diff>